<commit_message>
Added support for nullable types in column mappings.
</commit_message>
<xml_diff>
--- a/ExcelImports.Tests/TestFiles/Basic_Import.xlsx
+++ b/ExcelImports.Tests/TestFiles/Basic_Import.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>I</t>
   </si>
@@ -28,6 +28,9 @@
   </si>
   <si>
     <t>String 1</t>
+  </si>
+  <si>
+    <t>Another string</t>
   </si>
 </sst>
 </file>
@@ -367,7 +370,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
@@ -394,7 +397,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1">
-        <v>41268</v>
+        <v>41268.499652777777</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -405,7 +408,15 @@
         <v>654</v>
       </c>
       <c r="B3" s="1">
-        <v>41275.999305555553</v>
+        <v>41275</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>655</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>